<commit_message>
fix memory allocation start address
</commit_message>
<xml_diff>
--- a/docs/Reserved_Memory.xlsx
+++ b/docs/Reserved_Memory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteias\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F91B4FF-7AD8-48FC-8F79-EE69E6846B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21D23F9-5FD8-4D42-AC5D-824589841E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="510" windowWidth="29040" windowHeight="15990" xr2:uid="{D6997355-BD6F-49B1-AE1C-B333F470F503}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>Practice Codes Reserved Memory</t>
   </si>
   <si>
-    <t>Start Address: 0x81F00000</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>0xFFF</t>
+  </si>
+  <si>
+    <t>Start Address: 0x817F0000</t>
   </si>
 </sst>
 </file>
@@ -230,15 +230,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,7 +557,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,22 +577,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="B3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -608,14 +608,14 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>2</v>
+      <c r="D5" s="7" t="s">
+        <v>1</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -623,14 +623,14 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>13</v>
+      <c r="B6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -638,14 +638,14 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>14</v>
+      <c r="B7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -653,14 +653,14 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>15</v>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -668,14 +668,14 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -683,14 +683,14 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -698,14 +698,14 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -713,14 +713,14 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>22</v>
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -728,14 +728,14 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>23</v>
+      <c r="B13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -743,14 +743,14 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -758,14 +758,14 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -773,14 +773,14 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>

</xml_diff>

<commit_message>
update reserved memory ranges
</commit_message>
<xml_diff>
--- a/docs/Reserved_Memory.xlsx
+++ b/docs/Reserved_Memory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteias\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\sheep\github\gctGenerator\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9790C330-18A2-471B-AE04-2AC8C48F3D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CE5FEA-3720-44C0-8821-828E525E52A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="510" windowWidth="29040" windowHeight="15990" xr2:uid="{D6997355-BD6F-49B1-AE1C-B333F470F503}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="28800" windowHeight="15560" xr2:uid="{D6997355-BD6F-49B1-AE1C-B333F470F503}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
   <si>
     <t>Practice Codes Reserved Memory</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Ingame Timer: Stop Stopwatch  Flag</t>
   </si>
   <si>
-    <t>0x10D</t>
-  </si>
-  <si>
     <t>0xFFF</t>
   </si>
   <si>
@@ -136,6 +133,90 @@
   </si>
   <si>
     <t>0x13</t>
+  </si>
+  <si>
+    <t>0x94</t>
+  </si>
+  <si>
+    <t>0xA3</t>
+  </si>
+  <si>
+    <t>QF Timer: Coordinated of the Text box (LTRB)</t>
+  </si>
+  <si>
+    <t>0xA4</t>
+  </si>
+  <si>
+    <t>0xB0</t>
+  </si>
+  <si>
+    <t>0xB2</t>
+  </si>
+  <si>
+    <t>QF Timer: Stop at QFT Offset</t>
+  </si>
+  <si>
+    <t>QF Timer: Timer Format String</t>
+  </si>
+  <si>
+    <t>0xB3</t>
+  </si>
+  <si>
+    <t>QF Timer: Restart Flag</t>
+  </si>
+  <si>
+    <t>0xB4</t>
+  </si>
+  <si>
+    <t>0xB8</t>
+  </si>
+  <si>
+    <t>0xB7</t>
+  </si>
+  <si>
+    <t>0xBB</t>
+  </si>
+  <si>
+    <t>0xBC</t>
+  </si>
+  <si>
+    <t>0xBF</t>
+  </si>
+  <si>
+    <t>QF Timer: Duration of timer freeze (in frames)</t>
+  </si>
+  <si>
+    <t>QF Timer: Time to display if timer freeze  &gt; 0</t>
+  </si>
+  <si>
+    <t>QF Timer: (Unused)</t>
+  </si>
+  <si>
+    <t>QF Timer: Cumulative time of previous areas since last reset  (QFT Offset)</t>
+  </si>
+  <si>
+    <t>0xC0</t>
+  </si>
+  <si>
+    <t>0x93</t>
+  </si>
+  <si>
+    <t>0x110</t>
+  </si>
+  <si>
+    <t>QF Timer: Timer Textbox</t>
+  </si>
+  <si>
+    <t>0x10F</t>
+  </si>
+  <si>
+    <t>0xA50</t>
+  </si>
+  <si>
+    <t>0xA4F</t>
+  </si>
+  <si>
+    <t>Buffer</t>
   </si>
 </sst>
 </file>
@@ -165,7 +246,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +268,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -218,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -242,6 +329,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,19 +647,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46189971-4C8B-43DF-A9B2-D0E2994EAA14}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="48" style="1" customWidth="1"/>
+    <col min="4" max="4" width="62.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -578,7 +668,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="8" t="s">
         <v>0</v>
@@ -589,10 +679,10 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -600,7 +690,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -609,7 +699,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="6" t="s">
         <v>10</v>
@@ -624,7 +714,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="6" t="s">
         <v>2</v>
@@ -639,13 +729,13 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>5</v>
@@ -654,7 +744,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="6" t="s">
         <v>7</v>
@@ -669,13 +759,13 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>9</v>
@@ -684,7 +774,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="6" t="s">
         <v>14</v>
@@ -699,13 +789,13 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>19</v>
@@ -714,152 +804,272 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="6" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="6" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="6" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="6" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="6" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>19</v>
+        <v>41</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
+      <c r="B17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
+      <c r="B18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
+      <c r="B19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
+      <c r="B20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>60</v>
+      </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
+      <c r="B21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
+      <c r="B22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
+      <c r="B23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
+      <c r="B24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="4"/>
+      <c r="B25" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="4"/>
+      <c r="B27" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -868,6 +1078,6 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>